<commit_message>
fibonaaci optimal using DP
</commit_message>
<xml_diff>
--- a/Problems Summary.xlsx
+++ b/Problems Summary.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Done?</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>Check the reminder in hashtable. If not found, store value in the table else return the index</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>Fibonaaci</t>
+  </si>
+  <si>
+    <t>Store the computed sub-problem in hashTable. If the value is found in the hashTable, return else store it.</t>
   </si>
 </sst>
 </file>
@@ -834,7 +843,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -894,7 +903,18 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
@@ -1231,17 +1251,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d92cf942c19623f8ea37c5ae89e9e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ae4c53a902569674f13d354e575c07c" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1422,6 +1431,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1432,16 +1452,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3511A8E7-3D57-4C93-9399-7802901BCCB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD6F333A-FB7A-4713-AA13-3301CC37B3E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1460,6 +1470,16 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3511A8E7-3D57-4C93-9399-7802901BCCB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE30400F-CAE8-4146-AE00-683424BA2263}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
robot travelling in grid
</commit_message>
<xml_diff>
--- a/Problems Summary.xlsx
+++ b/Problems Summary.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Done?</t>
   </si>
@@ -123,6 +123,24 @@
   </si>
   <si>
     <t>Store the computed sub-problem in hashTable. If the value is found in the hashTable, return else store it.</t>
+  </si>
+  <si>
+    <t>DP, Recursion</t>
+  </si>
+  <si>
+    <t>Grid Traveller</t>
+  </si>
+  <si>
+    <t>O(n*m)</t>
+  </si>
+  <si>
+    <t>Identify the base cases. First solve the problem recursively(brute force) then add hash table to store the values.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-paths/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/fibonacci-number/</t>
   </si>
 </sst>
 </file>
@@ -221,7 +239,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -252,6 +270,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -843,7 +864,7 @@
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -909,6 +930,9 @@
       <c r="C5" t="s">
         <v>28</v>
       </c>
+      <c r="D5" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>
@@ -917,7 +941,21 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
@@ -1251,6 +1289,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d92cf942c19623f8ea37c5ae89e9e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ae4c53a902569674f13d354e575c07c" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1431,17 +1480,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1452,6 +1490,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3511A8E7-3D57-4C93-9399-7802901BCCB1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD6F333A-FB7A-4713-AA13-3301CC37B3E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1470,16 +1518,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3511A8E7-3D57-4C93-9399-7802901BCCB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE30400F-CAE8-4146-AE00-683424BA2263}">
   <ds:schemaRefs>

</xml_diff>